<commit_message>
more revisions, commit before pixel removal
</commit_message>
<xml_diff>
--- a/word_revision/Table3.xlsx
+++ b/word_revision/Table3.xlsx
@@ -354,7 +354,7 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>denote significant differences in the means for segments within each estuary (i.e., segments in an estuary with the same superscript are not significantly different). See Figs. 7 to 9 for spatial distribution of the results</t>
+      <t>denote significant differences in segment means. Segments with the same superscript are not significantly different. Multiple comparison tests are only within estuaries, not between estuaries. See Figs. 7 to 9 for spatial distribution of the results</t>
     </r>
   </si>
 </sst>
@@ -497,6 +497,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -507,9 +510,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -842,37 +842,37 @@
     <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:11" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
     </row>
     <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.35">
       <c r="A2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="H2" s="14" t="s">
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="H2" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
@@ -1409,19 +1409,19 @@
       </c>
     </row>
     <row r="21" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="13"/>
-      <c r="I21" s="13"/>
-      <c r="J21" s="13"/>
-      <c r="K21" s="13"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>

<commit_message>
updated text/figs/tabs with NA light removed if zc > z
</commit_message>
<xml_diff>
--- a/word_revision/Table3.xlsx
+++ b/word_revision/Table3.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
   <si>
     <t>OTB</t>
   </si>
@@ -365,7 +365,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,13 +414,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <i/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -462,14 +455,16 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -487,9 +482,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -497,20 +489,68 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -826,87 +866,92 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K21"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:K1"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" style="1" customWidth="1"/>
-    <col min="3" max="6" width="7.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="4.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="7.140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="6" width="6.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2" style="1" customWidth="1"/>
+    <col min="8" max="12" width="6.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="87" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:12" ht="72" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-    </row>
-    <row r="2" spans="1:11" ht="18.75" x14ac:dyDescent="0.35">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+    </row>
+    <row r="2" spans="1:12" ht="18.75" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="H2" s="15" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="H2" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6"/>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="G3" s="20"/>
+      <c r="H3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="J3" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="K3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="L3" s="20" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="3"/>
@@ -915,520 +960,567 @@
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
     </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1">
         <v>171</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="25">
         <v>0.21650610000000001</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="25">
         <v>0.4644741</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="25">
         <v>4.1782620000000001</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11">
-        <v>56.408459999999998</v>
-      </c>
-      <c r="I5" s="11">
-        <v>5.1607830000000003</v>
-      </c>
-      <c r="J5" s="11">
-        <v>19.509398000000001</v>
-      </c>
-      <c r="K5" s="11">
-        <v>91.696060000000003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G5" s="10"/>
+      <c r="H5" s="22">
+        <v>156</v>
+      </c>
+      <c r="I5" s="16">
+        <v>59.4</v>
+      </c>
+      <c r="J5" s="16">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K5" s="16">
+        <v>23.4</v>
+      </c>
+      <c r="L5" s="16">
+        <v>91.7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="1">
         <v>16</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D6" s="11">
+      <c r="D6" s="25">
         <v>0.41413040000000001</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="25">
         <v>0.37450879999999998</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="25">
         <v>0.94454830000000001</v>
       </c>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11">
-        <v>74.684920000000005</v>
-      </c>
-      <c r="I6" s="11">
-        <v>10.049412999999999</v>
-      </c>
-      <c r="J6" s="11">
-        <v>58.016669999999998</v>
-      </c>
-      <c r="K6" s="11">
-        <v>88.597840000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G6" s="18"/>
+      <c r="H6" s="23">
+        <v>16</v>
+      </c>
+      <c r="I6" s="19">
+        <v>74.7</v>
+      </c>
+      <c r="J6" s="19">
+        <v>8.6</v>
+      </c>
+      <c r="K6" s="19">
+        <v>58</v>
+      </c>
+      <c r="L6" s="19">
+        <v>88.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="10">
+      <c r="B7" s="9">
         <v>151</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="26">
         <v>0.26406160000000001</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="26">
         <v>1.6100057999999999</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="26">
         <v>2.8355413999999999</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12">
-        <v>46.350290000000001</v>
-      </c>
-      <c r="I7" s="12">
-        <v>6.397996</v>
-      </c>
-      <c r="J7" s="12">
-        <v>22.310746999999999</v>
-      </c>
-      <c r="K7" s="12">
-        <v>77.941909999999993</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G7" s="11"/>
+      <c r="H7" s="24">
+        <v>131</v>
+      </c>
+      <c r="I7" s="20">
+        <v>50.5</v>
+      </c>
+      <c r="J7" s="20">
+        <v>5.7</v>
+      </c>
+      <c r="K7" s="20">
+        <v>35.5</v>
+      </c>
+      <c r="L7" s="20">
+        <v>77.900000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C8" s="17"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="22"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+    </row>
+    <row r="9" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="1">
         <v>2</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="11">
+      <c r="D9" s="25">
         <v>0.36229709999999998</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="25">
         <v>0.95455310000000004</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="25">
         <v>1.0878954000000001</v>
       </c>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11">
-        <v>20.74577</v>
-      </c>
-      <c r="I9" s="11">
-        <v>7.5257699999999996</v>
-      </c>
-      <c r="J9" s="11">
-        <v>20.170309</v>
-      </c>
-      <c r="K9" s="11">
-        <v>21.32123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G9" s="10"/>
+      <c r="H9" s="22">
+        <v>17</v>
+      </c>
+      <c r="I9" s="16">
+        <v>20.7</v>
+      </c>
+      <c r="J9" s="16">
+        <v>7.5</v>
+      </c>
+      <c r="K9" s="16">
+        <v>7.5</v>
+      </c>
+      <c r="L9" s="16">
+        <v>30.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="1">
         <v>14</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="25">
         <v>0.31572430000000001</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="25">
         <v>0.92523789999999995</v>
       </c>
-      <c r="F10" s="11">
+      <c r="F10" s="25">
         <v>1.6005422</v>
       </c>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11">
-        <v>13.61896</v>
-      </c>
-      <c r="I10" s="11">
-        <v>6.4084859999999999</v>
-      </c>
-      <c r="J10" s="11">
-        <v>5.8381400000000001</v>
-      </c>
-      <c r="K10" s="11">
-        <v>24.73095</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G10" s="10"/>
+      <c r="H10" s="22">
+        <v>2</v>
+      </c>
+      <c r="I10" s="16">
+        <v>13.6</v>
+      </c>
+      <c r="J10" s="16">
+        <v>6.4</v>
+      </c>
+      <c r="K10" s="16">
+        <v>20.2</v>
+      </c>
+      <c r="L10" s="16">
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="25">
         <v>0.36258820000000003</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11" s="25">
         <v>1.5317681999999999</v>
       </c>
-      <c r="F11" s="11">
+      <c r="F11" s="25">
         <v>1.5815676000000001</v>
       </c>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11">
-        <v>9.1974300000000007</v>
-      </c>
-      <c r="I11" s="11">
-        <v>7.112158</v>
-      </c>
-      <c r="J11" s="11">
-        <v>6.0286590000000002</v>
-      </c>
-      <c r="K11" s="11">
-        <v>11.2212</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G11" s="10"/>
+      <c r="H11" s="22">
+        <v>3</v>
+      </c>
+      <c r="I11" s="16">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="J11" s="16">
+        <v>7.1</v>
+      </c>
+      <c r="K11" s="16">
+        <v>6</v>
+      </c>
+      <c r="L11" s="16">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="1">
         <v>4</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="11">
+      <c r="D12" s="25">
         <v>0.3625292</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="25">
         <v>0.96312010000000003</v>
       </c>
-      <c r="F12" s="11">
+      <c r="F12" s="25">
         <v>1.0162483</v>
       </c>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11">
-        <v>22.147359999999999</v>
-      </c>
-      <c r="I12" s="11">
-        <v>6.8960549999999996</v>
-      </c>
-      <c r="J12" s="11">
-        <v>19.330048999999999</v>
-      </c>
-      <c r="K12" s="11">
-        <v>24.321149999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G12" s="10"/>
+      <c r="H12" s="22">
+        <v>14</v>
+      </c>
+      <c r="I12" s="16">
+        <v>22.1</v>
+      </c>
+      <c r="J12" s="16">
+        <v>6.9</v>
+      </c>
+      <c r="K12" s="16">
+        <v>5.8</v>
+      </c>
+      <c r="L12" s="16">
+        <v>24.7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1">
         <v>17</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="25">
         <v>0.31846390000000002</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="25">
         <v>0.82741589999999998</v>
       </c>
-      <c r="F13" s="11">
+      <c r="F13" s="25">
         <v>1.0715477</v>
       </c>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11">
-        <v>20.0184</v>
-      </c>
-      <c r="I13" s="11">
-        <v>6.3726599999999998</v>
-      </c>
-      <c r="J13" s="11">
-        <v>7.4691010000000002</v>
-      </c>
-      <c r="K13" s="11">
-        <v>30.7378</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G13" s="10"/>
+      <c r="H13" s="22">
+        <v>1</v>
+      </c>
+      <c r="I13" s="16">
+        <v>20</v>
+      </c>
+      <c r="J13" s="16">
+        <v>6.4</v>
+      </c>
+      <c r="K13" s="16">
+        <v>24.1</v>
+      </c>
+      <c r="L13" s="16">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="25">
         <v>0.36572060000000001</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="25">
         <v>1.0297106</v>
       </c>
-      <c r="F14" s="11">
+      <c r="F14" s="25">
         <v>1.0297106</v>
       </c>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11">
-        <v>24.091329999999999</v>
-      </c>
-      <c r="I14" s="11">
-        <v>8.6487289999999994</v>
-      </c>
-      <c r="J14" s="11">
-        <v>24.091325999999999</v>
-      </c>
-      <c r="K14" s="11">
-        <v>24.091329999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G14" s="18"/>
+      <c r="H14" s="23">
+        <v>4</v>
+      </c>
+      <c r="I14" s="19">
+        <v>24.1</v>
+      </c>
+      <c r="J14" s="19">
+        <v>8.6</v>
+      </c>
+      <c r="K14" s="19">
+        <v>19.3</v>
+      </c>
+      <c r="L14" s="19">
+        <v>24.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="9">
         <v>6</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="26">
         <v>0.33067999999999997</v>
       </c>
-      <c r="E15" s="12">
+      <c r="E15" s="26">
         <v>0.77745039999999999</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="26">
         <v>0.96777899999999994</v>
       </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12">
-        <v>24.01859</v>
-      </c>
-      <c r="I15" s="12">
-        <v>6.6729580000000004</v>
-      </c>
-      <c r="J15" s="12">
-        <v>15.168393999999999</v>
-      </c>
-      <c r="K15" s="12">
-        <v>30.894410000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="G15" s="11"/>
+      <c r="H15" s="24">
+        <v>6</v>
+      </c>
+      <c r="I15" s="20">
+        <v>24</v>
+      </c>
+      <c r="J15" s="20">
+        <v>6.7</v>
+      </c>
+      <c r="K15" s="20">
+        <v>15.2</v>
+      </c>
+      <c r="L15" s="20">
+        <v>30.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-    </row>
-    <row r="17" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C16" s="17"/>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+    </row>
+    <row r="17" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B17" s="1">
         <v>22</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="25">
         <v>0.15884980000000001</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="25">
         <v>0.63782970000000005</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="25">
         <v>1.3229598</v>
       </c>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11">
-        <v>41.103580000000001</v>
-      </c>
-      <c r="I17" s="11">
-        <v>6.0084309999999999</v>
-      </c>
-      <c r="J17" s="11">
-        <v>17.696287999999999</v>
-      </c>
-      <c r="K17" s="11">
-        <v>50.812379999999997</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G17" s="10"/>
+      <c r="H17" s="22">
+        <v>19</v>
+      </c>
+      <c r="I17" s="16">
+        <v>43.2</v>
+      </c>
+      <c r="J17" s="16">
+        <v>6.9</v>
+      </c>
+      <c r="K17" s="16">
+        <v>17.7</v>
+      </c>
+      <c r="L17" s="16">
+        <v>50.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B18" s="1">
         <v>70</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="25">
         <v>0.129472</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="25">
         <v>0.82644379999999995</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="25">
         <v>1.5096202999999999</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11">
-        <v>39.098979999999997</v>
-      </c>
-      <c r="I18" s="11">
-        <v>4.838768</v>
-      </c>
-      <c r="J18" s="11">
-        <v>20.976942000000001</v>
-      </c>
-      <c r="K18" s="11">
-        <v>58.693820000000002</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="G18" s="10"/>
+      <c r="H18" s="22">
+        <v>56</v>
+      </c>
+      <c r="I18" s="16">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="J18" s="16">
+        <v>5.6</v>
+      </c>
+      <c r="K18" s="16">
+        <v>22.5</v>
+      </c>
+      <c r="L18" s="16">
+        <v>58.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="1">
         <v>73</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="25">
         <v>0.12645210000000001</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="25">
         <v>1.0572760999999999</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F19" s="25">
         <v>1.6332139999999999</v>
       </c>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11">
-        <v>36.37453</v>
-      </c>
-      <c r="I19" s="11">
-        <v>4.718248</v>
-      </c>
-      <c r="J19" s="11">
-        <v>11.750893</v>
-      </c>
-      <c r="K19" s="11">
-        <v>50.194499999999998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="G19" s="10"/>
+      <c r="H19" s="22">
+        <v>62</v>
+      </c>
+      <c r="I19" s="16">
+        <v>36.5</v>
+      </c>
+      <c r="J19" s="16">
+        <v>5.5</v>
+      </c>
+      <c r="K19" s="16">
+        <v>15.2</v>
+      </c>
+      <c r="L19" s="16">
+        <v>50.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="29">
         <v>87</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="31">
         <v>0.13155130000000001</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="31">
         <v>0.49749169999999998</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F20" s="31">
         <v>1.0827316</v>
       </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11">
-        <v>48.739019999999996</v>
-      </c>
-      <c r="I20" s="11">
-        <v>4.9055730000000004</v>
-      </c>
-      <c r="J20" s="11">
-        <v>31.520123000000002</v>
-      </c>
-      <c r="K20" s="11">
-        <v>77.433909999999997</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="G20" s="32"/>
+      <c r="H20" s="33">
+        <v>83</v>
+      </c>
+      <c r="I20" s="34">
+        <v>47.7</v>
+      </c>
+      <c r="J20" s="34">
+        <v>5.6</v>
+      </c>
+      <c r="K20" s="34">
+        <v>31.5</v>
+      </c>
+      <c r="L20" s="34">
+        <v>77.400000000000006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="14"/>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
-      <c r="K21" s="14"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A21:K21"/>
-    <mergeCell ref="H2:K2"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A21:L21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>